<commit_message>
Output adc result successfully
Output adc result successfully
</commit_message>
<xml_diff>
--- a/TouchGFX/assets/texts/texts.xlsx
+++ b/TouchGFX/assets/texts/texts.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="53">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -171,13 +171,17 @@
   </si>
   <si>
     <t xml:space="preserve">Left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -449,127 +453,127 @@
     </border>
   </borders>
   <cellStyleXfs count="82">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" xfId="0" applyAlignment="0"/>
   </cellStyleXfs>
   <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="81" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyFill="1" applyAlignment="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -577,91 +581,91 @@
   <cellStyles count="82">
     <cellStyle name="Accent1" xfId="81" builtinId="29"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 10" xfId="1"/>
-    <cellStyle name="Normal 10 2" xfId="2"/>
-    <cellStyle name="Normal 11" xfId="3"/>
-    <cellStyle name="Normal 12" xfId="4"/>
-    <cellStyle name="Normal 13" xfId="5"/>
-    <cellStyle name="Normal 14" xfId="6"/>
-    <cellStyle name="Normal 14 2" xfId="7"/>
-    <cellStyle name="Normal 15" xfId="8"/>
-    <cellStyle name="Normal 16" xfId="9"/>
-    <cellStyle name="Normal 16 2" xfId="10"/>
-    <cellStyle name="Normal 16 3" xfId="11"/>
-    <cellStyle name="Normal 17 2" xfId="12"/>
-    <cellStyle name="Normal 17 3" xfId="13"/>
-    <cellStyle name="Normal 2" xfId="14"/>
-    <cellStyle name="Normal 2 2" xfId="15"/>
-    <cellStyle name="Normal 2 3" xfId="16"/>
-    <cellStyle name="Normal 2 4" xfId="17"/>
-    <cellStyle name="Normal 2 5" xfId="18"/>
-    <cellStyle name="Normal 2 6" xfId="19"/>
-    <cellStyle name="Normal 2 7" xfId="20"/>
-    <cellStyle name="Normal 2 8" xfId="21"/>
-    <cellStyle name="Normal 2 9" xfId="22"/>
-    <cellStyle name="Normal 22" xfId="23"/>
-    <cellStyle name="Normal 22 10" xfId="24"/>
-    <cellStyle name="Normal 22 11" xfId="25"/>
-    <cellStyle name="Normal 22 12" xfId="26"/>
-    <cellStyle name="Normal 22 13" xfId="27"/>
-    <cellStyle name="Normal 22 14" xfId="28"/>
-    <cellStyle name="Normal 22 15" xfId="29"/>
-    <cellStyle name="Normal 22 16" xfId="30"/>
-    <cellStyle name="Normal 22 17" xfId="31"/>
-    <cellStyle name="Normal 22 18" xfId="32"/>
-    <cellStyle name="Normal 22 2" xfId="33"/>
-    <cellStyle name="Normal 22 3" xfId="34"/>
-    <cellStyle name="Normal 22 4" xfId="35"/>
-    <cellStyle name="Normal 22 5" xfId="36"/>
-    <cellStyle name="Normal 22 6" xfId="37"/>
-    <cellStyle name="Normal 22 7" xfId="38"/>
-    <cellStyle name="Normal 22 8" xfId="39"/>
-    <cellStyle name="Normal 22 9" xfId="40"/>
-    <cellStyle name="Normal 23 10" xfId="41"/>
-    <cellStyle name="Normal 23 11" xfId="42"/>
-    <cellStyle name="Normal 23 12" xfId="43"/>
-    <cellStyle name="Normal 23 13" xfId="44"/>
-    <cellStyle name="Normal 23 14" xfId="45"/>
-    <cellStyle name="Normal 23 15" xfId="46"/>
-    <cellStyle name="Normal 23 16" xfId="47"/>
-    <cellStyle name="Normal 23 17" xfId="48"/>
-    <cellStyle name="Normal 23 18" xfId="49"/>
-    <cellStyle name="Normal 23 2" xfId="50"/>
-    <cellStyle name="Normal 23 3" xfId="51"/>
-    <cellStyle name="Normal 23 4" xfId="52"/>
-    <cellStyle name="Normal 23 5" xfId="53"/>
-    <cellStyle name="Normal 23 6" xfId="54"/>
-    <cellStyle name="Normal 23 7" xfId="55"/>
-    <cellStyle name="Normal 23 8" xfId="56"/>
-    <cellStyle name="Normal 23 9" xfId="57"/>
-    <cellStyle name="Normal 25 10" xfId="58"/>
-    <cellStyle name="Normal 25 11" xfId="59"/>
-    <cellStyle name="Normal 25 12" xfId="60"/>
-    <cellStyle name="Normal 25 13" xfId="61"/>
-    <cellStyle name="Normal 25 14" xfId="62"/>
-    <cellStyle name="Normal 25 15" xfId="63"/>
-    <cellStyle name="Normal 25 16" xfId="64"/>
-    <cellStyle name="Normal 25 17" xfId="65"/>
-    <cellStyle name="Normal 25 2" xfId="66"/>
-    <cellStyle name="Normal 25 3" xfId="67"/>
-    <cellStyle name="Normal 25 4" xfId="68"/>
-    <cellStyle name="Normal 25 5" xfId="69"/>
-    <cellStyle name="Normal 25 6" xfId="70"/>
-    <cellStyle name="Normal 25 7" xfId="71"/>
-    <cellStyle name="Normal 25 8" xfId="72"/>
-    <cellStyle name="Normal 25 9" xfId="73"/>
-    <cellStyle name="Normal 3" xfId="74"/>
-    <cellStyle name="Normal 4" xfId="75"/>
-    <cellStyle name="Normal 5" xfId="76"/>
-    <cellStyle name="Normal 6" xfId="77"/>
-    <cellStyle name="Normal 7" xfId="78"/>
-    <cellStyle name="Normal 8" xfId="79"/>
-    <cellStyle name="Normal 9" xfId="80"/>
+    <cellStyle name="Normal 10" xfId="1" builtinId="0"/>
+    <cellStyle name="Normal 10 2" xfId="2" builtinId="0"/>
+    <cellStyle name="Normal 11" xfId="3" builtinId="0"/>
+    <cellStyle name="Normal 12" xfId="4" builtinId="0"/>
+    <cellStyle name="Normal 13" xfId="5" builtinId="0"/>
+    <cellStyle name="Normal 14" xfId="6" builtinId="0"/>
+    <cellStyle name="Normal 14 2" xfId="7" builtinId="0"/>
+    <cellStyle name="Normal 15" xfId="8" builtinId="0"/>
+    <cellStyle name="Normal 16" xfId="9" builtinId="0"/>
+    <cellStyle name="Normal 16 2" xfId="10" builtinId="0"/>
+    <cellStyle name="Normal 16 3" xfId="11" builtinId="0"/>
+    <cellStyle name="Normal 17 2" xfId="12" builtinId="0"/>
+    <cellStyle name="Normal 17 3" xfId="13" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="14" builtinId="0"/>
+    <cellStyle name="Normal 2 2" xfId="15" builtinId="0"/>
+    <cellStyle name="Normal 2 3" xfId="16" builtinId="0"/>
+    <cellStyle name="Normal 2 4" xfId="17" builtinId="0"/>
+    <cellStyle name="Normal 2 5" xfId="18" builtinId="0"/>
+    <cellStyle name="Normal 2 6" xfId="19" builtinId="0"/>
+    <cellStyle name="Normal 2 7" xfId="20" builtinId="0"/>
+    <cellStyle name="Normal 2 8" xfId="21" builtinId="0"/>
+    <cellStyle name="Normal 2 9" xfId="22" builtinId="0"/>
+    <cellStyle name="Normal 22" xfId="23" builtinId="0"/>
+    <cellStyle name="Normal 22 10" xfId="24" builtinId="0"/>
+    <cellStyle name="Normal 22 11" xfId="25" builtinId="0"/>
+    <cellStyle name="Normal 22 12" xfId="26" builtinId="0"/>
+    <cellStyle name="Normal 22 13" xfId="27" builtinId="0"/>
+    <cellStyle name="Normal 22 14" xfId="28" builtinId="0"/>
+    <cellStyle name="Normal 22 15" xfId="29" builtinId="0"/>
+    <cellStyle name="Normal 22 16" xfId="30" builtinId="0"/>
+    <cellStyle name="Normal 22 17" xfId="31" builtinId="0"/>
+    <cellStyle name="Normal 22 18" xfId="32" builtinId="0"/>
+    <cellStyle name="Normal 22 2" xfId="33" builtinId="0"/>
+    <cellStyle name="Normal 22 3" xfId="34" builtinId="0"/>
+    <cellStyle name="Normal 22 4" xfId="35" builtinId="0"/>
+    <cellStyle name="Normal 22 5" xfId="36" builtinId="0"/>
+    <cellStyle name="Normal 22 6" xfId="37" builtinId="0"/>
+    <cellStyle name="Normal 22 7" xfId="38" builtinId="0"/>
+    <cellStyle name="Normal 22 8" xfId="39" builtinId="0"/>
+    <cellStyle name="Normal 22 9" xfId="40" builtinId="0"/>
+    <cellStyle name="Normal 23 10" xfId="41" builtinId="0"/>
+    <cellStyle name="Normal 23 11" xfId="42" builtinId="0"/>
+    <cellStyle name="Normal 23 12" xfId="43" builtinId="0"/>
+    <cellStyle name="Normal 23 13" xfId="44" builtinId="0"/>
+    <cellStyle name="Normal 23 14" xfId="45" builtinId="0"/>
+    <cellStyle name="Normal 23 15" xfId="46" builtinId="0"/>
+    <cellStyle name="Normal 23 16" xfId="47" builtinId="0"/>
+    <cellStyle name="Normal 23 17" xfId="48" builtinId="0"/>
+    <cellStyle name="Normal 23 18" xfId="49" builtinId="0"/>
+    <cellStyle name="Normal 23 2" xfId="50" builtinId="0"/>
+    <cellStyle name="Normal 23 3" xfId="51" builtinId="0"/>
+    <cellStyle name="Normal 23 4" xfId="52" builtinId="0"/>
+    <cellStyle name="Normal 23 5" xfId="53" builtinId="0"/>
+    <cellStyle name="Normal 23 6" xfId="54" builtinId="0"/>
+    <cellStyle name="Normal 23 7" xfId="55" builtinId="0"/>
+    <cellStyle name="Normal 23 8" xfId="56" builtinId="0"/>
+    <cellStyle name="Normal 23 9" xfId="57" builtinId="0"/>
+    <cellStyle name="Normal 25 10" xfId="58" builtinId="0"/>
+    <cellStyle name="Normal 25 11" xfId="59" builtinId="0"/>
+    <cellStyle name="Normal 25 12" xfId="60" builtinId="0"/>
+    <cellStyle name="Normal 25 13" xfId="61" builtinId="0"/>
+    <cellStyle name="Normal 25 14" xfId="62" builtinId="0"/>
+    <cellStyle name="Normal 25 15" xfId="63" builtinId="0"/>
+    <cellStyle name="Normal 25 16" xfId="64" builtinId="0"/>
+    <cellStyle name="Normal 25 17" xfId="65" builtinId="0"/>
+    <cellStyle name="Normal 25 2" xfId="66" builtinId="0"/>
+    <cellStyle name="Normal 25 3" xfId="67" builtinId="0"/>
+    <cellStyle name="Normal 25 4" xfId="68" builtinId="0"/>
+    <cellStyle name="Normal 25 5" xfId="69" builtinId="0"/>
+    <cellStyle name="Normal 25 6" xfId="70" builtinId="0"/>
+    <cellStyle name="Normal 25 7" xfId="71" builtinId="0"/>
+    <cellStyle name="Normal 25 8" xfId="72" builtinId="0"/>
+    <cellStyle name="Normal 25 9" xfId="73" builtinId="0"/>
+    <cellStyle name="Normal 3" xfId="74" builtinId="0"/>
+    <cellStyle name="Normal 4" xfId="75" builtinId="0"/>
+    <cellStyle name="Normal 5" xfId="76" builtinId="0"/>
+    <cellStyle name="Normal 6" xfId="77" builtinId="0"/>
+    <cellStyle name="Normal 7" xfId="78" builtinId="0"/>
+    <cellStyle name="Normal 8" xfId="79" builtinId="0"/>
+    <cellStyle name="Normal 9" xfId="80" builtinId="0"/>
   </cellStyles>
   <dxfs count="17">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -681,8 +685,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -704,8 +708,8 @@
       </border>
     </dxf>
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
+      <alignment horizontal="left"/>
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -727,7 +731,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -752,7 +756,7 @@
       <font>
         <b/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left/>
         <right style="thin">
           <color indexed="64"/>
@@ -779,7 +783,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -802,7 +806,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -820,7 +824,7 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
+      <border>
         <left style="medium">
           <color indexed="64"/>
         </left>
@@ -896,7 +900,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="TableStyleLight9 2" pivot="0" count="7">
+    <tableStyle name="TableStyleLight9 2" pivot="0" table="0" count="7">
       <tableStyleElement type="wholeTable" dxfId="16"/>
       <tableStyleElement type="firstColumn" dxfId="15"/>
       <tableStyleElement type="lastColumn" dxfId="14"/>
@@ -907,44 +911,44 @@
     </tableStyle>
   </tableStyles>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" totalsRowShown="0" tableBorderDxfId="9">
-  <sortState ref="B4:E6">
-    <sortCondition descending="1" ref="B3:B65536"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="B3:J100" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" tableBorderDxfId="9">
+  <sortState columnSort="0" caseSensitive="0" sortMethod="none" ref="B4:E6">
+    <sortCondition descending="1" sortBy="value" ref="B3:B65536" iconSet="3Arrows"/>
   </sortState>
   <tableColumns count="9">
-    <tableColumn id="1" name="Typography Name"/>
-    <tableColumn id="2" name="Font"/>
-    <tableColumn id="3" name="Size"/>
-    <tableColumn id="4" name="Bpp"/>
-    <tableColumn id="5" name="Fallback Character"/>
-    <tableColumn id="6" name="Wildcard Characters"/>
-    <tableColumn id="9" name="Widget Wildcard Characters"/>
-    <tableColumn id="7" name="Wildcard Ranges"/>
-    <tableColumn id="8" name="Ellipsis Character"/>
+    <tableColumn id="1" name="Typography Name" totalsRowFunction="none"/>
+    <tableColumn id="2" name="Font" totalsRowFunction="none"/>
+    <tableColumn id="3" name="Size" totalsRowFunction="none"/>
+    <tableColumn id="4" name="Bpp" totalsRowFunction="none"/>
+    <tableColumn id="5" name="Fallback Character" totalsRowFunction="none"/>
+    <tableColumn id="6" name="Wildcard Characters" totalsRowFunction="none"/>
+    <tableColumn id="9" name="Widget Wildcard Characters" totalsRowFunction="none"/>
+    <tableColumn id="7" name="Wildcard Ranges" totalsRowFunction="none"/>
+    <tableColumn id="8" name="Ellipsis Character" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" totalsRowShown="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table3" displayName="Table3" ref="L4:P10" tableType="worksheet" headerRowCount="1" insertRow="0" insertRowShift="0" totalsRowShown="0" published="0" headerRowDxfId="8" headerRowBorderDxfId="7" tableBorderDxfId="6" totalsRowBorderDxfId="5">
   <tableColumns count="5">
-    <tableColumn id="1" name="Column" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Example 1" dataDxfId="2"/>
-    <tableColumn id="4" name="Example 2" dataDxfId="1"/>
-    <tableColumn id="5" name="Example 3" dataDxfId="0"/>
+    <tableColumn id="1" name="Column" totalsRowFunction="none" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" totalsRowFunction="none" dataDxfId="3"/>
+    <tableColumn id="3" name="Example 1" totalsRowFunction="none" dataDxfId="2"/>
+    <tableColumn id="4" name="Example 2" totalsRowFunction="none" dataDxfId="1"/>
+    <tableColumn id="5" name="Example 3" totalsRowFunction="none"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -994,8 +998,8 @@
     <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:ea/>
+        <a:cs/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -1029,8 +1033,8 @@
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
+        <a:ea/>
+        <a:cs/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
@@ -1065,169 +1069,108 @@
     </a:fontScheme>
     <a:fmtScheme name="Office">
       <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="50000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
+            </gs>
+            <gs pos="35000">
               <a:schemeClr val="phClr">
                 <a:tint val="37000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:tint val="15000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
+            </gs>
+            <gs pos="80000">
               <a:schemeClr val="phClr">
                 <a:shade val="93000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="94000"/>
                 <a:satMod val="135000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill rotWithShape="1">
+      </a:fillStyleLst>
+      <a:bgFillStyleLst>
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="40000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
+            </gs>
+            <gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
                 <a:shade val="99000"/>
                 <a:satMod val="350000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="20000"/>
                 <a:satMod val="255000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
+        <a:gradFill flip="none" rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0">
+            <gs>
               <a:schemeClr val="phClr">
                 <a:tint val="80000"/>
                 <a:satMod val="300000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
+            </gs>
+            <gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="30000"/>
                 <a:satMod val="200000"/>
               </a:schemeClr>
-            </a:gs>
+            </gs>
           </a:gsLst>
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
       </a:bgFillStyleLst>
+      <a:lnStyleLst/>
+      <a:effectStyleLst/>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
@@ -1238,24 +1181,23 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
-          <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1270,7 +1212,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
       <a:lstStyle/>
     </a:spDef>
     <a:lnDef>
@@ -1280,24 +1222,23 @@
           <a:ext cx="1" cy="1"/>
         </a:xfrm>
         <a:custGeom>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:avLst/>
           <a:gdLst/>
-          <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst/>
         </a:custGeom>
         <a:solidFill>
-          <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="090000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="9"/>
+          <a:srgbClr val="090000"/>
         </a:solidFill>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:srgbClr xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="400000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+            <a:srgbClr val="400000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:round/>
-          <a:headEnd type="none" w="med" len="med"/>
-          <a:tailEnd type="none" w="med" len="med"/>
+          <a:headEnd w="med" len="med"/>
+          <a:tailEnd w="med" len="med"/>
         </a:ln>
         <a:effectLst/>
         <a:extLst>
@@ -1312,7 +1253,7 @@
           </a:ext>
         </a:extLst>
       </a:spPr>
-      <a:bodyPr vertOverflow="clip" wrap="square" lIns="18288" tIns="0" rIns="0" bIns="0" upright="1"/>
+      <a:bodyPr rot="0" vertOverflow="clip" vert="horz" wrap="square" lIns="18288" rtlCol="0" anchor="t" upright="1"/>
       <a:lstStyle/>
     </a:lnDef>
   </a:objectDefaults>
@@ -1412,12 +1353,18 @@
       <c r="F4" t="s">
         <v>17</v>
       </c>
-      <c r="G4"/>
+      <c r="G4" t="s">
+        <v>48</v>
+      </c>
       <c r="H4" t="s">
         <v>44</v>
       </c>
-      <c r="I4"/>
-      <c r="J4"/>
+      <c r="I4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J4" t="s">
+        <v>48</v>
+      </c>
       <c r="L4" s="4" t="s">
         <v>9</v>
       </c>
@@ -1601,13 +1548,13 @@
     </row>
     <row r="4">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
         <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="E4" t="s">
         <v>47</v>
@@ -1618,13 +1565,13 @@
     </row>
     <row r="5">
       <c r="B5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
         <v>47</v>

</xml_diff>